<commit_message>
Added reading attrition schemes (v0.1.2)
* Added the functions that read the attrition schemes from an Excel file.
* Added basic unit tests to validate these functions.
</commit_message>
<xml_diff>
--- a/test/base/catalogue.xlsx
+++ b/test/base/catalogue.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="76">
   <si>
     <t xml:space="preserve">General catalogue information</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attrition 1</t>
   </si>
   <si>
     <t xml:space="preserve">Is fixed?</t>
@@ -573,7 +576,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -614,7 +617,7 @@
       </c>
       <c r="B4" s="6" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(INDIRECT(CONCATENATE(Misc!A5,"A2")),0,0,OFFSET(B4,0,1))),0,0),0)-1,OFFSET(B4,0,1))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="7" t="n">
         <v>1000</v>
@@ -700,8 +703,8 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -754,20 +757,34 @@
       <c r="K2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>12</v>
+      </c>
       <c r="C3" s="10" t="n">
         <f aca="true">_xlfn.FLOOR.MATH(IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(C3,0,1,1,200)),0,0),0)-1,200)/2)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="11"/>
+      <c r="E3" s="11" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F3" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="H3" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3" s="11" t="n">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
@@ -879,19 +896,19 @@
         <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -899,83 +916,83 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="10" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(E2,0,1,1,200)),0,0),0)-1,200)</f>
         <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="10" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(E3,0,1,1,200)),0,0),0)-1,200)</f>
         <v>4</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="10" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(E4,0,1,1,200)),0,0),0)-1,200)</f>
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -983,152 +1000,152 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9"/>
       <c r="B5" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" s="10" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(E5,0,1,1,200)),0,0),0)-1,200)</f>
         <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9"/>
       <c r="B6" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="15" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(E6,0,1,1,200)),0,0),0)-1,200)</f>
         <v>4</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9"/>
       <c r="B7" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="15" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(E7,0,1,1,200)),0,0),0)-1,200)</f>
         <v>4</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
       <c r="B8" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" s="15" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(E8,0,1,1,200)),0,0),0)-1,200)</f>
         <v>2</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
       <c r="B9" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" s="15" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(E9,0,1,1,200)),0,0),0)-1,200)</f>
         <v>2</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9"/>
       <c r="B10" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" s="15" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(E10,0,1,1,200)),0,0),0)-1,200)</f>
         <v>3</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1171,7 +1188,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1182,23 +1199,23 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" s="16" t="n">
         <f aca="true">IFERROR(MATCH(TRUE(),INDEX(ISBLANK(OFFSET(B5,3,0,5*INDIRECT(CONCATENATE(Misc!A4,"B5")))),0,0),0)-1,5*INDIRECT(CONCATENATE(Misc!A4,"B5")))</f>
@@ -1211,10 +1228,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,7 +1239,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,7 +1247,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,7 +1255,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,36 +1331,36 @@
         <v>8</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" s="17" t="n">
         <v>12</v>
@@ -1356,33 +1373,33 @@
         <v>3</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" s="17" t="n">
         <v>12</v>
@@ -1395,33 +1412,33 @@
         <v>3</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D4" s="17" t="n">
         <v>12</v>
@@ -1434,33 +1451,33 @@
         <v>3</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" s="17" t="n">
         <v>12</v>
@@ -1473,33 +1490,33 @@
         <v>3</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="17" t="n">
         <v>12</v>
@@ -1512,33 +1529,33 @@
         <v>3</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" s="17" t="n">
         <v>12</v>
@@ -1551,33 +1568,33 @@
         <v>3</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="17" t="n">
         <v>12</v>
@@ -1590,21 +1607,21 @@
         <v>1</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="17" t="n">
         <v>12</v>
@@ -1617,21 +1634,21 @@
         <v>1</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="17" t="n">
         <v>12</v>
@@ -1644,21 +1661,21 @@
         <v>1</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="17" t="n">
         <v>12</v>
@@ -1671,10 +1688,10 @@
         <v>1</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1724,13 +1741,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E9" type="decimal">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:C9" type="list">
       <formula1>Misc!$B$1:$B$2</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E9" type="decimal">
-      <formula1>0</formula1>
-      <formula2>1</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D9" type="decimal">
       <formula1>0</formula1>
@@ -1778,92 +1795,92 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9"/>
       <c r="B7" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
       <c r="B8" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
       <c r="B9" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9"/>
       <c r="B10" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9"/>
       <c r="B11" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
       <c r="B12" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
       <c r="B13" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1908,13 +1925,13 @@
         <v>1000</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1923,13 +1940,13 @@
         <v>.</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,7 +1955,7 @@
         <v>1000</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>